<commit_message>
Corrected XLS init templates
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal-fr_FR/init.xlsx
+++ b/Resources/fixtures/minimal-fr_FR/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="270">
   <si>
     <t>en_US</t>
   </si>
@@ -274,9 +274,6 @@
     <t>Code article</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>global</t>
   </si>
   <si>
@@ -289,9 +286,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
@@ -340,33 +334,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>conversion_units-Area</t>
-  </si>
-  <si>
-    <t>conversion_units-Binary</t>
-  </si>
-  <si>
-    <t>conversion_units-Frequency</t>
-  </si>
-  <si>
-    <t>conversion_units-Length</t>
-  </si>
-  <si>
-    <t>conversion_units-Power</t>
-  </si>
-  <si>
-    <t>conversion_units-Speed</t>
-  </si>
-  <si>
-    <t>conversion_units-Temperature</t>
-  </si>
-  <si>
-    <t>conversion_units-Volume</t>
-  </si>
-  <si>
-    <t>conversion_units-Weight</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -418,39 +385,21 @@
     <t>pim_catalog_textarea</t>
   </si>
   <si>
-    <t>Text area</t>
-  </si>
-  <si>
     <t>pim_catalog_multiselect</t>
   </si>
   <si>
-    <t>Multiple select</t>
-  </si>
-  <si>
     <t>pim_catalog_simpleselect</t>
   </si>
   <si>
-    <t>Simple select</t>
-  </si>
-  <si>
     <t>pim_catalog_price_collection</t>
   </si>
   <si>
-    <t>Price collection</t>
-  </si>
-  <si>
     <t>pim_catalog_number</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>pim_catalog_boolean</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
     <t>pim_catalog_date</t>
   </si>
   <si>
@@ -460,9 +409,6 @@
     <t>pim_catalog_file</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>pim_catalog_image</t>
   </si>
   <si>
@@ -470,9 +416,6 @@
   </si>
   <si>
     <t>pim_catalog_metric</t>
-  </si>
-  <si>
-    <t>Metric</t>
   </si>
   <si>
     <t>unit</t>
@@ -1015,9 +958,6 @@
     <t>Propriétés du canal</t>
   </si>
   <si>
-    <t>Unités de mesure par défaut</t>
-  </si>
-  <si>
     <t>Code du canal</t>
   </si>
   <si>
@@ -1031,30 +971,6 @@
   </si>
   <si>
     <t>Arbre de categories</t>
-  </si>
-  <si>
-    <t>Surface</t>
-  </si>
-  <si>
-    <t>Binaire</t>
-  </si>
-  <si>
-    <t>Fréquence</t>
-  </si>
-  <si>
-    <t>Longueurr</t>
-  </si>
-  <si>
-    <t>Puissance</t>
-  </si>
-  <si>
-    <t>Vitesse</t>
-  </si>
-  <si>
-    <t>Température</t>
-  </si>
-  <si>
-    <t>Poids</t>
   </si>
   <si>
     <t>Code de la catégorie</t>
@@ -1103,6 +1019,50 @@
   </si>
   <si>
     <t>Décimales autorisées</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ne pas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>enregistrer ce fichier avec une extension autre que xlsx</t>
+    </r>
+  </si>
+  <si>
+    <t>Identifiant</t>
+  </si>
+  <si>
+    <t>Texte</t>
+  </si>
+  <si>
+    <t>Zone de texte</t>
+  </si>
+  <si>
+    <t>Select multiple</t>
+  </si>
+  <si>
+    <t>Select simple</t>
+  </si>
+  <si>
+    <t>Collection de prix</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Booléen</t>
+  </si>
+  <si>
+    <t>Fichier</t>
+  </si>
+  <si>
+    <t>Mesure</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1266,15 +1226,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1308,6 +1259,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1492,8 +1449,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -1535,8 +1492,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -1951,9 +1908,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1961,143 +1920,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>199</v>
+      <c r="A1" s="22" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
-        <v>200</v>
+      <c r="B3" s="21" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
-        <v>201</v>
+      <c r="B5" s="23" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
-        <v>202</v>
+      <c r="B6" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="26" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>204</v>
+      <c r="B7" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>283</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>208</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>210</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="26" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>218</v>
+      <c r="B28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="24" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>223</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>224</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +2074,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2122,10 +2086,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2133,103 +2097,103 @@
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2259,10 +2223,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2270,79 +2234,79 @@
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2372,7 +2336,7 @@
   <sheetData>
     <row r="1" spans="1:1024" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1"/>
@@ -2382,704 +2346,704 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B68" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B69" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B75" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B77" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B78" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B79" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B80" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B81" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B84" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B85" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B86" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B88" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B89" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3096,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3106,15 +3070,15 @@
     <col min="2" max="3" width="24.7109375"/>
     <col min="4" max="4" width="23.7109375"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="19"/>
-    <col min="7" max="7" width="14" style="19"/>
-    <col min="8" max="8" width="13" style="19"/>
-    <col min="9" max="9" width="25.85546875" style="19"/>
-    <col min="10" max="10" width="25.140625" style="19"/>
+    <col min="6" max="6" width="19.7109375" style="16"/>
+    <col min="7" max="7" width="14" style="16"/>
+    <col min="8" max="8" width="13" style="16"/>
+    <col min="9" max="9" width="25.85546875" style="16"/>
+    <col min="10" max="10" width="25.140625" style="16"/>
     <col min="11" max="11" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" style="19"/>
-    <col min="13" max="13" width="34.5703125" style="19" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" style="19" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" style="16"/>
+    <col min="13" max="13" width="34.5703125" style="16" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" style="16" customWidth="1"/>
     <col min="15" max="15" width="20.42578125"/>
     <col min="16" max="16" width="19.28515625"/>
     <col min="17" max="17" width="25.5703125" customWidth="1"/>
@@ -3130,7 +3094,7 @@
     <col min="28" max="28" width="21"/>
     <col min="29" max="29" width="22"/>
     <col min="30" max="30" width="34.5703125" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" style="19"/>
+    <col min="31" max="31" width="14.85546875" style="16"/>
     <col min="32" max="40" width="13.42578125"/>
     <col min="41" max="41" width="16.85546875"/>
     <col min="42" max="42" width="19.140625"/>
@@ -3148,7 +3112,7 @@
     <row r="1" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="AY1"/>
       <c r="AZ1"/>
@@ -3173,141 +3137,141 @@
       <c r="BA2"/>
       <c r="BB2"/>
     </row>
-    <row r="4" spans="1:54" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+    <row r="4" spans="1:54" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
+      <c r="D4" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
       <c r="AE4" s="7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="S5" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="T5" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="U5" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="V5" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="W5" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="X5" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y5" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="Z5" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="AA5" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="AB5" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="AC5" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="AD5" s="25" t="s">
         <v>233</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="J5" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="M5" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="N5" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="P5" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="S5" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="T5" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="U5" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="V5" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="W5" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="X5" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y5" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z5" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA5" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="AB5" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="AC5" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="AD5" s="28" t="s">
-        <v>252</v>
       </c>
       <c r="AE5" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:54" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -3315,7 +3279,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>8</v>
@@ -3323,31 +3287,31 @@
       <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="17" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="17" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="9" t="s">
@@ -3398,7 +3362,7 @@
       <c r="AD6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AE6" s="23"/>
+      <c r="AE6" s="20"/>
       <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6"/>
@@ -3412,34 +3376,34 @@
         <v>36</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="19">
+      <c r="F7" s="16">
         <v>1</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="18">
         <v>0</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="18">
         <v>1</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="18">
         <v>1</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="18">
         <v>0</v>
       </c>
       <c r="K7" s="11"/>
-      <c r="L7" s="21">
+      <c r="L7" s="18">
         <v>0</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="18">
         <v>1</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="18">
         <v>1</v>
       </c>
       <c r="O7" s="11"/>
@@ -3457,7 +3421,7 @@
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
-      <c r="AE7" s="21">
+      <c r="AE7" s="18">
         <v>1</v>
       </c>
       <c r="AF7" s="11"/>
@@ -3480,7 +3444,7 @@
       <c r="AW7" s="11"/>
       <c r="AX7" s="11"/>
       <c r="AY7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="BA7" s="2">
         <v>1</v>
@@ -3488,45 +3452,45 @@
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>42</v>
+        <v>261</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="19">
+        <v>37</v>
+      </c>
+      <c r="F8" s="16">
         <v>2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <v>0</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="16">
         <v>0</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="16">
         <v>1</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="16">
         <v>0</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="16">
         <v>0</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="16">
         <v>1</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="16">
         <v>1</v>
       </c>
-      <c r="AE8" s="19">
+      <c r="AE8" s="16">
         <v>1</v>
       </c>
     </row>
@@ -3603,15 +3567,6 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>attribute_types!$B$3:$B$14</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>D7:D8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>attribute_groups!$A$4:$A$257</xm:f>
           </x14:formula1>
           <xm:sqref>E7:E1048576</xm:sqref>
@@ -3627,6 +3582,12 @@
             <xm:f>metric_units!$B$3:$B$89</xm:f>
           </x14:formula1>
           <xm:sqref>AA7:AA1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attribute_types!$B$3:$B$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3651,23 +3612,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="31"/>
       <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24.4" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3678,18 +3639,18 @@
         <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3718,41 +3679,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="A1" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3773,10 +3734,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3786,119 +3747,53 @@
     <col min="3" max="3" width="17.140625" style="11"/>
     <col min="4" max="4" width="20.140625" style="11"/>
     <col min="5" max="5" width="21.85546875" style="11" customWidth="1"/>
-    <col min="6" max="14" width="17.140625" style="11"/>
-    <col min="15" max="1025" width="17.140625"/>
+    <col min="6" max="1016" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -3909,43 +3804,15 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>77</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:N1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="C4:E4">
@@ -3957,66 +3824,6 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$3:$B$20</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$21:$B$26</xm:f>
-          </x14:formula1>
-          <xm:sqref>G4:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$27:$B$31</xm:f>
-          </x14:formula1>
-          <xm:sqref>H4:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$32:$B$45</xm:f>
-          </x14:formula1>
-          <xm:sqref>I4:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$46:$B$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>J4:J1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$51:$B$58</xm:f>
-          </x14:formula1>
-          <xm:sqref>K4:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$59:$B$63</xm:f>
-          </x14:formula1>
-          <xm:sqref>L4:L1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$64:$B$78</xm:f>
-          </x14:formula1>
-          <xm:sqref>M4:M1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>metric_units!$B$79:$B$89</xm:f>
-          </x14:formula1>
-          <xm:sqref>N4:N1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4036,23 +3843,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="31"/>
       <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
@@ -4060,10 +3867,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4071,7 +3878,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4105,17 +3912,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -4123,12 +3930,12 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4136,7 +3943,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4161,69 +3968,69 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41" style="12" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>279</v>
+    <row r="2" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>251</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>192</v>
+        <v>172</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>194</v>
+        <v>174</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>196</v>
+        <v>176</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>198</v>
+        <v>178</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4253,10 +4060,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4264,18 +4071,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added attributes tab and corrected validation on french init file
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal-fr_FR/init.xlsx
+++ b/Resources/fixtures/minimal-fr_FR/init.xlsx
@@ -4,25 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="6990" tabRatio="226" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4005" tabRatio="226"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
-    <sheet name="family main" sheetId="1" r:id="rId2"/>
-    <sheet name="attribute_groups" sheetId="2" r:id="rId3"/>
-    <sheet name="options" sheetId="3" r:id="rId4"/>
-    <sheet name="channels" sheetId="4" r:id="rId5"/>
-    <sheet name="categories" sheetId="5" r:id="rId6"/>
-    <sheet name="group_types" sheetId="11" r:id="rId7"/>
-    <sheet name="association_types" sheetId="14" r:id="rId8"/>
-    <sheet name="choices" sheetId="9" state="hidden" r:id="rId9"/>
-    <sheet name="attribute_types" sheetId="6" state="hidden" r:id="rId10"/>
-    <sheet name="metric_types" sheetId="7" state="hidden" r:id="rId11"/>
-    <sheet name="metric_units" sheetId="8" state="hidden" r:id="rId12"/>
+    <sheet name="attributes" sheetId="15" r:id="rId2"/>
+    <sheet name="family main" sheetId="1" r:id="rId3"/>
+    <sheet name="attribute_groups" sheetId="2" r:id="rId4"/>
+    <sheet name="options" sheetId="3" r:id="rId5"/>
+    <sheet name="channels" sheetId="4" r:id="rId6"/>
+    <sheet name="categories" sheetId="5" r:id="rId7"/>
+    <sheet name="group_types" sheetId="11" r:id="rId8"/>
+    <sheet name="association_types" sheetId="14" r:id="rId9"/>
+    <sheet name="choices" sheetId="9" state="hidden" r:id="rId10"/>
+    <sheet name="attribute_types" sheetId="6" state="hidden" r:id="rId11"/>
+    <sheet name="metric_types" sheetId="7" state="hidden" r:id="rId12"/>
+    <sheet name="metric_units" sheetId="8" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'family main'!$C$6:$BA$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AX$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$AZ$9</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
     <definedName name="date_choices">choices!$C$1:$C$3</definedName>
     <definedName name="validation_choices">choices!$B$1:$B$3</definedName>
@@ -37,20 +39,7 @@
     <author>SMILE</author>
   </authors>
   <commentList>
-    <comment ref="AE4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insérer 1 si l'attribut est requis pour cette famille et ce canal</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC5" authorId="0">
+    <comment ref="AA5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD5" authorId="0">
+    <comment ref="AB5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,6 +93,73 @@
     <author>SMILE</author>
   </authors>
   <commentList>
+    <comment ref="AD4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insérer 1 si l'attribut est requis pour cette famille et ce canal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Spécifier le nom des locales, séparées par ","
+Par exemple : "en_US, fr_FR"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Inscrire les extensions permises, séparées par une ","
+Par exemple : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Spécifie le nombre de caractères à taper pour avoir une liste d'options, pour les attributs de type select.
+Cette option doit être utilisée si de nombreuses options sont proposées</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SMILE</author>
+  </authors>
+  <commentList>
     <comment ref="C2" authorId="0">
       <text>
         <r>
@@ -121,7 +177,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>SMILE</author>
@@ -161,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="272">
   <si>
     <t>en_US</t>
   </si>
@@ -194,9 +250,6 @@
   </si>
   <si>
     <t>sort_order</t>
-  </si>
-  <si>
-    <t>required</t>
   </si>
   <si>
     <t>unique</t>
@@ -871,9 +924,6 @@
     <t>Ordre de tri</t>
   </si>
   <si>
-    <t>Requis*</t>
-  </si>
-  <si>
     <t>Unique*</t>
   </si>
   <si>
@@ -995,21 +1045,6 @@
   </si>
   <si>
     <t>Après avoir modifié les informations de cet onglet, vous pourrez avoir à modifier les onglets "family" afin de corriger les codes des canaux</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Si un attribut est présent dans plusieurs familles, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>les colonnes roses et bleues (propriétés et labels de l'attribut) ne devront pas être remplies qu'une fois</t>
-    </r>
   </si>
   <si>
     <t>Extensions autorisées</t>
@@ -1063,6 +1098,45 @@
   </si>
   <si>
     <t>Mesure</t>
+  </si>
+  <si>
+    <t>Attributs partagés / non liés à une famille</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>L'onglet attributes peut être utilisé pour les informations relatives aux attributs communs à plusieurs familles, ou non affectés à des familles.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si un attribut est présent dans plusieurs familles, ou est défini dans un onglet attributes, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>les colonnes roses et bleues (propriétés et labels de l'attribut) ne devront pas être remplies qu'une fois</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cet onglet peut être dupliqué pour séparer la liste en plusieurs parties. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Le titre de l'onglet devra commencer par "attributes"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1185,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1266,6 +1340,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1908,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1921,147 +1996,168 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="23"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="32" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>189</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="23" t="s">
-        <v>254</v>
+      <c r="B29" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="21" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="21" t="s">
+    <row r="45" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="21" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2070,6 +2166,51 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2086,10 +2227,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2097,103 +2238,103 @@
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
         <v>82</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2206,7 +2347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -2223,10 +2364,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2234,79 +2375,79 @@
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2319,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ89"/>
   <sheetViews>
@@ -2336,7 +2477,7 @@
   <sheetData>
     <row r="1" spans="1:1024" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="9"/>
       <c r="AMJ1"/>
@@ -2346,704 +2487,704 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AMJ2"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B86" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3058,10 +3199,494 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:AY8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" style="16" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="26.42578125" customWidth="1"/>
+    <col min="26" max="26" width="23.140625" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="34.5703125" customWidth="1"/>
+    <col min="48" max="48" width="9.140625" style="2"/>
+    <col min="49" max="49" width="9.140625" style="3"/>
+    <col min="50" max="51" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="AV1"/>
+      <c r="AW1"/>
+      <c r="AX1"/>
+      <c r="AY1"/>
+    </row>
+    <row r="2" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+    </row>
+    <row r="4" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+    </row>
+    <row r="5" spans="1:51" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="S5" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="T5" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="U5" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="V5" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="W5" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="X5" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z5" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA5" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB5" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1</v>
+      </c>
+      <c r="G7" s="18">
+        <v>1</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="18">
+        <v>0</v>
+      </c>
+      <c r="K7" s="18">
+        <v>1</v>
+      </c>
+      <c r="L7" s="18">
+        <v>1</v>
+      </c>
+      <c r="M7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="11"/>
+      <c r="AP7" s="11"/>
+      <c r="AQ7" s="11"/>
+      <c r="AR7" s="11"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="11"/>
+      <c r="AV7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="16">
+        <v>2</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0</v>
+      </c>
+      <c r="K8" s="16">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:AB4"/>
+  </mergeCells>
+  <dataValidations count="17">
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7:AA1048576"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="Q7:R1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B1048576">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="Z7:Z1048576 AB7:AB1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:U1048576">
+      <formula1>date_choices</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N7:N1048576">
+      <formula1>validation_choices</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:L1048576 P7:P1048576 S7:T1048576 F7:H1048576">
+      <formula1>boolean_choices</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="E7">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7 AP7">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
+      <formula1>datetype</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD7">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
+      <formula1>$Q$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
+      <formula1>validation_type</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
+      <formula1>0</formula1>
+      <formula2>200</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7:AM7 AR7:AT7">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attribute_types!$B$3:$B$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>metric_units!$B$3:$B$89</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y7:Y1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>metric_types!$B$3:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>X7:X1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attribute_groups!$A$4:$A$257</xm:f>
+          </x14:formula1>
+          <xm:sqref>D7:D1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BA8"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3071,55 +3696,54 @@
     <col min="4" max="4" width="23.7109375"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="16"/>
-    <col min="7" max="7" width="14" style="16"/>
-    <col min="8" max="8" width="13" style="16"/>
-    <col min="9" max="9" width="25.85546875" style="16"/>
-    <col min="10" max="10" width="25.140625" style="16"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" style="16"/>
-    <col min="13" max="13" width="34.5703125" style="16" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" style="16" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125"/>
-    <col min="16" max="16" width="19.28515625"/>
-    <col min="17" max="17" width="25.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625"/>
-    <col min="19" max="19" width="16.5703125"/>
-    <col min="20" max="20" width="19"/>
-    <col min="21" max="21" width="21.42578125" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375"/>
-    <col min="23" max="24" width="13.42578125"/>
-    <col min="25" max="25" width="19.85546875"/>
-    <col min="26" max="26" width="20.42578125" customWidth="1"/>
-    <col min="27" max="27" width="26.42578125" customWidth="1"/>
-    <col min="28" max="28" width="21"/>
-    <col min="29" max="29" width="22"/>
-    <col min="30" max="30" width="34.5703125" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" style="16"/>
-    <col min="32" max="40" width="13.42578125"/>
-    <col min="41" max="41" width="16.85546875"/>
-    <col min="42" max="42" width="19.140625"/>
-    <col min="43" max="43" width="16.28515625"/>
-    <col min="44" max="46" width="13.42578125"/>
-    <col min="47" max="47" width="19.140625"/>
-    <col min="48" max="50" width="18.140625"/>
-    <col min="51" max="51" width="0" style="2" hidden="1"/>
-    <col min="52" max="52" width="0" style="3" hidden="1"/>
-    <col min="53" max="53" width="0" style="2" hidden="1"/>
-    <col min="54" max="54" width="17.140625" style="2"/>
-    <col min="55" max="1025" width="17.140625"/>
+    <col min="7" max="7" width="13" style="16"/>
+    <col min="8" max="8" width="25.85546875" style="16"/>
+    <col min="9" max="9" width="25.140625" style="16"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="16"/>
+    <col min="12" max="12" width="34.5703125" style="16" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125"/>
+    <col min="15" max="15" width="19.28515625"/>
+    <col min="16" max="16" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625"/>
+    <col min="18" max="18" width="16.5703125"/>
+    <col min="19" max="19" width="19"/>
+    <col min="20" max="20" width="21.42578125" customWidth="1"/>
+    <col min="21" max="21" width="18.7109375"/>
+    <col min="22" max="23" width="13.42578125"/>
+    <col min="24" max="24" width="19.85546875"/>
+    <col min="25" max="25" width="20.42578125" customWidth="1"/>
+    <col min="26" max="26" width="26.42578125" customWidth="1"/>
+    <col min="27" max="27" width="21"/>
+    <col min="28" max="28" width="22"/>
+    <col min="29" max="29" width="34.5703125" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" style="16"/>
+    <col min="31" max="39" width="13.42578125"/>
+    <col min="40" max="40" width="16.85546875"/>
+    <col min="41" max="41" width="19.140625"/>
+    <col min="42" max="42" width="16.28515625"/>
+    <col min="43" max="45" width="13.42578125"/>
+    <col min="46" max="46" width="19.140625"/>
+    <col min="47" max="49" width="18.140625"/>
+    <col min="50" max="50" width="0" style="2" hidden="1"/>
+    <col min="51" max="51" width="0" style="3" hidden="1"/>
+    <col min="52" max="52" width="0" style="2" hidden="1"/>
+    <col min="53" max="53" width="17.140625" style="2"/>
+    <col min="54" max="1024" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>208</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="AX1"/>
       <c r="AY1"/>
       <c r="AZ1"/>
       <c r="BA1"/>
-      <c r="BB1"/>
-    </row>
-    <row r="2" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3132,19 +3756,19 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
-      <c r="BB2"/>
-    </row>
-    <row r="4" spans="1:54" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:53" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -3171,107 +3795,103 @@
       <c r="AA4" s="30"/>
       <c r="AB4" s="30"/>
       <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD4" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="C5" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>208</v>
-      </c>
       <c r="D5" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="F5" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="G5" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="H5" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="I5" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="J5" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="K5" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="L5" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="M5" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="N5" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="O5" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="P5" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="R5" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="S5" s="25" t="s">
+      <c r="T5" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="U5" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="V5" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="T5" s="25" t="s">
+      <c r="W5" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="U5" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="V5" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="W5" s="25" t="s">
+      <c r="X5" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="X5" s="25" t="s">
+      <c r="Y5" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="Y5" s="25" t="s">
+      <c r="Z5" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="AA5" s="25" t="s">
+      <c r="AB5" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="AC5" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="AB5" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="AC5" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="AD5" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AD5" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -3279,7 +3899,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>8</v>
@@ -3299,10 +3919,10 @@
       <c r="I6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="17" t="s">
@@ -3311,7 +3931,7 @@
       <c r="M6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="9" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="9" t="s">
@@ -3359,54 +3979,27 @@
       <c r="AC6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AX6"/>
       <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6"/>
-      <c r="BB6"/>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>1</v>
-      </c>
-      <c r="I7" s="18">
-        <v>1</v>
-      </c>
-      <c r="J7" s="18">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
-      <c r="M7" s="18">
-        <v>1</v>
-      </c>
-      <c r="N7" s="18">
-        <v>1</v>
-      </c>
-      <c r="O7" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="11"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -3420,10 +4013,10 @@
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="18">
+      <c r="AD7" s="18">
         <v>1</v>
       </c>
+      <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
@@ -3442,92 +4035,56 @@
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="11"/>
-      <c r="AX7" s="11"/>
-      <c r="AY7" s="2" t="s">
+      <c r="AX7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>38</v>
-      </c>
-      <c r="BA7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>39</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="16">
-        <v>2</v>
-      </c>
-      <c r="G8" s="16">
-        <v>0</v>
-      </c>
-      <c r="H8" s="16">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16">
-        <v>1</v>
-      </c>
-      <c r="J8" s="16">
-        <v>0</v>
-      </c>
-      <c r="L8" s="16">
-        <v>0</v>
-      </c>
-      <c r="M8" s="16">
-        <v>1</v>
-      </c>
-      <c r="N8" s="16">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="16">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="AD8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AD4"/>
+    <mergeCell ref="D4:AC4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7:AP7 AU7:AW7">
+  <dataValidations count="18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7:AO7 AT7:AV7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
-      <formula1>$S$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
+      <formula1>$R$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7">
-      <formula1>#REF!</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ7 AS7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7 AR7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3535,29 +4092,36 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:J1048576 L7:N1048576 R7:R1048576 B7:B1048576 U7:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:M1048576 Q7:Q1048576 B7:B1048576 T7:U1048576 G7:I1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576"/>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576 AB7:AB1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AA7:AA1048576 AC7:AC1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1048576">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB7:AB1048576"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3575,13 +4139,13 @@
           <x14:formula1>
             <xm:f>metric_types!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>Z7:Z1048576</xm:sqref>
+          <xm:sqref>Y7:Y1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>metric_units!$B$3:$B$89</xm:f>
           </x14:formula1>
-          <xm:sqref>AA7:AA1048576</xm:sqref>
+          <xm:sqref>Z7:Z1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
@@ -3595,7 +4159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3613,7 +4177,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="13" t="s">
@@ -3622,13 +4186,13 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24.4" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3639,18 +4203,18 @@
         <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3662,7 +4226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3680,7 +4244,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3690,30 +4254,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3732,7 +4296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3752,7 +4316,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3761,19 +4325,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
@@ -3781,16 +4345,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3804,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>2</v>
@@ -3827,7 +4391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3844,7 +4408,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="13" t="s">
@@ -3853,13 +4417,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
@@ -3867,10 +4431,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3878,7 +4442,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3897,7 +4461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -3913,16 +4477,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -3930,12 +4494,12 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3943,7 +4507,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3963,7 +4527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -3979,7 +4543,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="27" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>5</v>
@@ -3987,10 +4551,10 @@
     </row>
     <row r="2" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -3998,39 +4562,39 @@
         <v>6</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>172</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>174</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>178</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4043,49 +4607,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>